<commit_message>
Updated BOM and core servo gear.
</commit_message>
<xml_diff>
--- a/Documents/BillofMaterials.xlsx
+++ b/Documents/BillofMaterials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Jack the Ripper Bot</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>M2 socket cap, ?mm</t>
+  </si>
+  <si>
+    <t>GWS S125 1T 2BB Sail Winch servo</t>
   </si>
 </sst>
 </file>
@@ -229,8 +232,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D29" totalsRowShown="0">
-  <autoFilter ref="A4:D29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D30" totalsRowShown="0">
+  <autoFilter ref="A4:D30"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Quantity"/>
     <tableColumn id="2" name="Description"/>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +611,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -625,21 +628,19 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,10 +648,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,7 +659,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,10 +670,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,10 +678,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -699,32 +700,32 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -732,13 +733,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,21 +744,27 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,7 +772,7 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,7 +780,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,7 +788,7 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,18 +796,26 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId1"/>
     <hyperlink ref="D10" r:id="rId2"/>
-    <hyperlink ref="D12" r:id="rId3"/>
-    <hyperlink ref="D13" r:id="rId4"/>
-    <hyperlink ref="D19" r:id="rId5"/>
-    <hyperlink ref="D21" r:id="rId6"/>
-    <hyperlink ref="D22" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId3"/>
+    <hyperlink ref="D14" r:id="rId4"/>
+    <hyperlink ref="D20" r:id="rId5"/>
+    <hyperlink ref="D22" r:id="rId6"/>
+    <hyperlink ref="D23" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>

</xml_diff>

<commit_message>
Updated bill of materials. Created list of what M2/M3 bolt are used where. Added more Ideas for Improvements. Colored hub retainer.
</commit_message>
<xml_diff>
--- a/Documents/BillofMaterials.xlsx
+++ b/Documents/BillofMaterials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Jack the Ripper Bot</t>
   </si>
@@ -132,9 +132,6 @@
     <t>http://www.amazon.co.uk/dp/B004ND4632/ref=pe_385721_37038051_pe_217191_31005151_3p_M3T1_dp_1</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>PLA or ABS plastic</t>
   </si>
   <si>
@@ -144,13 +141,34 @@
     <t>M2 nuts</t>
   </si>
   <si>
-    <t>M3 socket cap, ?mm</t>
-  </si>
-  <si>
-    <t>M2 socket cap, ?mm</t>
-  </si>
-  <si>
     <t>GWS S125 1T 2BB Sail Winch servo</t>
+  </si>
+  <si>
+    <t>M8 threaded rod, 220mm long</t>
+  </si>
+  <si>
+    <t>M3 washers</t>
+  </si>
+  <si>
+    <t>608ZZ Bearing</t>
+  </si>
+  <si>
+    <t>M3 socket cap, 12mm</t>
+  </si>
+  <si>
+    <t>M3 socket cap, 14mm</t>
+  </si>
+  <si>
+    <t>M3 socket cap, 16mm</t>
+  </si>
+  <si>
+    <t>M3 socket cap, 18mm</t>
+  </si>
+  <si>
+    <t>M2 socket cap, 10mm</t>
+  </si>
+  <si>
+    <t>M2 socket cap, 14mm</t>
   </si>
 </sst>
 </file>
@@ -232,8 +250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D30" totalsRowShown="0">
-  <autoFilter ref="A4:D30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D36" totalsRowShown="0">
+  <autoFilter ref="A4:D36"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Quantity"/>
     <tableColumn id="2" name="Description"/>
@@ -531,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,56 +589,50 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,30 +640,33 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,10 +674,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -670,7 +685,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,10 +696,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -689,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -711,32 +726,32 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,13 +759,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,64 +770,123 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
-    <hyperlink ref="D10" r:id="rId2"/>
-    <hyperlink ref="D13" r:id="rId3"/>
-    <hyperlink ref="D14" r:id="rId4"/>
-    <hyperlink ref="D20" r:id="rId5"/>
-    <hyperlink ref="D22" r:id="rId6"/>
-    <hyperlink ref="D23" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId2"/>
+    <hyperlink ref="D14" r:id="rId3"/>
+    <hyperlink ref="D15" r:id="rId4"/>
+    <hyperlink ref="D21" r:id="rId5"/>
+    <hyperlink ref="D23" r:id="rId6"/>
+    <hyperlink ref="D24" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>

</xml_diff>

<commit_message>
Added circuit diagram. Updated BOM.
</commit_message>
<xml_diff>
--- a/Documents/BillofMaterials.xlsx
+++ b/Documents/BillofMaterials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Jack the Ripper Bot</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>2 way 0.1 inch molex connector</t>
+  </si>
+  <si>
+    <t>2 pin PCB header</t>
   </si>
 </sst>
 </file>
@@ -256,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D37" totalsRowShown="0">
-  <autoFilter ref="A4:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D38" totalsRowShown="0">
+  <autoFilter ref="A4:D38"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Quantity"/>
     <tableColumn id="2" name="Description"/>
@@ -555,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +892,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>51</v>
@@ -901,6 +904,14 @@
       </c>
       <c r="B37" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>